<commit_message>
add test data and home page tests and methods to home page
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Data.xlsx
+++ b/src/test/resources/data/Data.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mahmoud\iti_testing\TrainingTestAutomation\Woodmart-kids\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2969074-8369-4BD5-B01A-4B9F31D98AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21214FF-2294-4175-9E91-ADB203DAD768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="3" r:id="rId1"/>
     <sheet name="login" sheetId="1" r:id="rId2"/>
+    <sheet name="lostPassword" sheetId="4" r:id="rId3"/>
+    <sheet name="categoryNames" sheetId="5" r:id="rId4"/>
+    <sheet name="productsNames" sheetId="6" r:id="rId5"/>
+    <sheet name="postsNames" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="51">
   <si>
     <t>userName</t>
   </si>
@@ -119,13 +123,73 @@
   </si>
   <si>
     <t>Unknown email address. Check again or try your username.</t>
+  </si>
+  <si>
+    <t>Password reset email has been sent.</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>Invalid username or email.</t>
+  </si>
+  <si>
+    <t>abcd@iti.com</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Toys</t>
+  </si>
+  <si>
+    <t>Leggings</t>
+  </si>
+  <si>
+    <t>Jumpers</t>
+  </si>
+  <si>
+    <t>Growsuits</t>
+  </si>
+  <si>
+    <t>Dresses</t>
+  </si>
+  <si>
+    <t>Accessories</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>3 Pack Baby Socks</t>
+  </si>
+  <si>
+    <t>Basic Rib Legging</t>
+  </si>
+  <si>
+    <t>Post Name</t>
+  </si>
+  <si>
+    <t>How to choose a baby growsuit &amp; onesie</t>
+  </si>
+  <si>
+    <t>Types of baby rashes and how to effectively treat them</t>
+  </si>
+  <si>
+    <t>How to choose a sleeping bag for your little one</t>
+  </si>
+  <si>
+    <t>Safely administering pain relief to your little one</t>
+  </si>
+  <si>
+    <t>Why choose organic cotton for your baby</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +216,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -174,7 +244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -189,6 +259,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -608,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,4 +810,204 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3CEA32-3119-424A-AD84-6DD57FE2A3FA}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{1EBF0771-4D1E-41AC-9AAF-D4DC5590A7BA}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{C1311F7A-2260-4EBA-B19B-9039BCD9B270}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75306103-3AD1-4587-ACD9-B8DCD4545159}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DBB6BA-2453-48FE-8B81-7F1D252FCA3F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E552492-DBA6-4BB8-BC7E-197D254B633F}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add contact us tests and some edits in listeners , base test and ContactUsPage classes
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Data.xlsx
+++ b/src/test/resources/data/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mahmoud\iti_testing\TrainingTestAutomation\Woodmart-kids\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21214FF-2294-4175-9E91-ADB203DAD768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23589600-350F-4B22-A4FB-266E177FA509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="categoryNames" sheetId="5" r:id="rId4"/>
     <sheet name="productsNames" sheetId="6" r:id="rId5"/>
     <sheet name="postsNames" sheetId="7" r:id="rId6"/>
+    <sheet name="contact" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="63">
   <si>
     <t>userName</t>
   </si>
@@ -50,9 +52,6 @@
     <t>iti@iti.com</t>
   </si>
   <si>
-    <t>result</t>
-  </si>
-  <si>
     <t>Success</t>
   </si>
   <si>
@@ -183,13 +182,52 @@
   </si>
   <si>
     <t>Why choose organic cotton for your baby</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last  Name</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>Thank you for your message. It has been sent.</t>
+  </si>
+  <si>
+    <t>One or more fields have an error. Please check and try again.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">first name and last name contain space </t>
+  </si>
+  <si>
+    <t>..</t>
+  </si>
+  <si>
+    <t>iti@iti</t>
+  </si>
+  <si>
+    <t>iti@.com</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Hi , this is a wonderful website</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,14 +245,6 @@
       <color theme="8"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
@@ -240,9 +270,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -255,18 +284,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -548,131 +576,123 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>7</v>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>9</v>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
-        <v>16</v>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>17</v>
+      <c r="D4" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>11</v>
+      <c r="D6" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>9</v>
+      <c r="D7" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{8E35B5B5-287A-4ECA-84F5-D6FDC6C16E30}"/>
-    <hyperlink ref="B6" r:id="rId2" xr:uid="{E7456C59-FFDF-4924-A3F3-50BDE8B22593}"/>
-    <hyperlink ref="B8" r:id="rId3" xr:uid="{69015178-B203-4324-9472-D1D3ED942FDA}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{88367C9E-D71D-43A5-AD29-FBDE87C0E185}"/>
-    <hyperlink ref="B3" r:id="rId5" xr:uid="{A77D1BC2-6A72-4026-B8D8-3BCD9955DCB7}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{D6467CFC-FBE5-426E-B4F6-48570C918381}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -701,7 +721,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
@@ -712,24 +732,24 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
@@ -737,7 +757,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
@@ -746,7 +766,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -756,58 +776,52 @@
       <c r="B7" s="3">
         <v>30215230</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>25</v>
+      <c r="C7" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>27</v>
+      <c r="C8" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="3">
         <v>30215230</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="C10" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{9A134EB7-F39B-45D6-8B24-0D2DFF1E360E}"/>
-    <hyperlink ref="A9" r:id="rId2" xr:uid="{86E210D7-2ABD-413F-8D5A-4AD0698BA0F4}"/>
-    <hyperlink ref="A10" r:id="rId3" xr:uid="{9B21E9F0-A655-4D0A-B6D3-FBBE3A85FD96}"/>
-    <hyperlink ref="A11" r:id="rId4" xr:uid="{93723091-A912-4B97-8F5E-8ED6F956AAC8}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -817,7 +831,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,7 +845,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
@@ -839,38 +853,34 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{1EBF0771-4D1E-41AC-9AAF-D4DC5590A7BA}"/>
-    <hyperlink ref="A5" r:id="rId2" xr:uid="{C1311F7A-2260-4EBA-B19B-9039BCD9B270}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -890,37 +900,37 @@
   <sheetData>
     <row r="1" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -944,18 +954,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -967,7 +977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E552492-DBA6-4BB8-BC7E-197D254B633F}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -978,36 +988,246 @@
   <sheetData>
     <row r="1" spans="1:1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="4" spans="1:1" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="5" spans="1:1" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="6" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A91842D-8BFD-42C4-B5AC-04E2D42130BE}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" customWidth="1"/>
+    <col min="6" max="6" width="36.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C3" s="3"/>
+      <c r="E3" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC979B5-DE00-4264-9D5B-F48CC73FC465}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edits some pages and tests(scroll to)
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Data.xlsx
+++ b/src/test/resources/data/Data.xlsx
@@ -8,19 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mahmoud\iti_testing\TrainingTestAutomation\Woodmart-kids\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23589600-350F-4B22-A4FB-266E177FA509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4DDE78-6D01-40F4-8206-E6554BBA9EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="register" sheetId="3" r:id="rId1"/>
+    <sheet name="register" sheetId="9" r:id="rId1"/>
     <sheet name="login" sheetId="1" r:id="rId2"/>
     <sheet name="lostPassword" sheetId="4" r:id="rId3"/>
     <sheet name="categoryNames" sheetId="5" r:id="rId4"/>
     <sheet name="productsNames" sheetId="6" r:id="rId5"/>
     <sheet name="postsNames" sheetId="7" r:id="rId6"/>
     <sheet name="contact" sheetId="8" r:id="rId7"/>
-    <sheet name="Sheet2" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -169,9 +168,6 @@
     <t>Post Name</t>
   </si>
   <si>
-    <t>How to choose a baby growsuit &amp; onesie</t>
-  </si>
-  <si>
     <t>Types of baby rashes and how to effectively treat them</t>
   </si>
   <si>
@@ -181,9 +177,6 @@
     <t>Safely administering pain relief to your little one</t>
   </si>
   <si>
-    <t>Why choose organic cotton for your baby</t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -221,6 +214,12 @@
   </si>
   <si>
     <t>Hi , this is a wonderful website</t>
+  </si>
+  <si>
+    <t>Why choose organic cotton for your baby?</t>
+  </si>
+  <si>
+    <t>How to choose a baby growsuit &amp; onesie?</t>
   </si>
 </sst>
 </file>
@@ -273,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -292,6 +291,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -572,22 +577,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2729F86-694D-4847-83E6-AC1BEB240E45}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC979B5-DE00-4264-9D5B-F48CC73FC465}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -597,8 +602,8 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>60</v>
+      <c r="D1" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
@@ -615,7 +620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -629,7 +634,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -641,7 +646,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -649,11 +654,11 @@
       <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -667,7 +672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -681,14 +686,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -721,7 +726,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
@@ -845,7 +850,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
@@ -978,7 +983,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,27 +998,27 @@
     </row>
     <row r="2" spans="1:1" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1027,7 +1032,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,19 +1047,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1062,22 +1067,22 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C3" s="3"/>
       <c r="E3" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
@@ -1089,10 +1094,10 @@
         <v>5</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
@@ -1100,66 +1105,66 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
@@ -1173,10 +1178,10 @@
         <v>5</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
@@ -1184,16 +1189,16 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
@@ -1201,33 +1206,19 @@
         <v>4</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC979B5-DE00-4264-9D5B-F48CC73FC465}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
edits some pages and add some wishlist tests
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Data.xlsx
+++ b/src/test/resources/data/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mahmoud\iti_testing\TrainingTestAutomation\Woodmart-kids\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4DDE78-6D01-40F4-8206-E6554BBA9EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4ABBB3D-F293-4B48-856C-E6EF4E058E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="9" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="productsNames" sheetId="6" r:id="rId5"/>
     <sheet name="postsNames" sheetId="7" r:id="rId6"/>
     <sheet name="contact" sheetId="8" r:id="rId7"/>
+    <sheet name="productsNames (2)" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="65">
   <si>
     <t>userName</t>
   </si>
@@ -220,6 +221,12 @@
   </si>
   <si>
     <t>How to choose a baby growsuit &amp; onesie?</t>
+  </si>
+  <si>
+    <t>Small Rainbow Jumper</t>
+  </si>
+  <si>
+    <t>CFrangipani Embroidered Dress</t>
   </si>
 </sst>
 </file>
@@ -1031,7 +1038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A91842D-8BFD-42C4-B5AC-04E2D42130BE}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -1221,4 +1228,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C670E76-5AAF-41AD-B6C2-06048ED546A3}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add end-to-end test and faker data class
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Data.xlsx
+++ b/src/test/resources/data/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mahmoud\iti_testing\TrainingTestAutomation\Woodmart-kids\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4ABBB3D-F293-4B48-856C-E6EF4E058E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1008B0-FDD7-492C-BA84-45162E2161F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="58">
   <si>
     <t>userName</t>
   </si>
@@ -94,12 +94,6 @@
     <t>iti289@iti.com</t>
   </si>
   <si>
-    <t>iti_5</t>
-  </si>
-  <si>
-    <t>iti_5@iti.com</t>
-  </si>
-  <si>
     <t>Error: Username is required.</t>
   </si>
   <si>
@@ -142,18 +136,6 @@
     <t>Toys</t>
   </si>
   <si>
-    <t>Leggings</t>
-  </si>
-  <si>
-    <t>Jumpers</t>
-  </si>
-  <si>
-    <t>Growsuits</t>
-  </si>
-  <si>
-    <t>Dresses</t>
-  </si>
-  <si>
     <t>Accessories</t>
   </si>
   <si>
@@ -172,12 +154,6 @@
     <t>Types of baby rashes and how to effectively treat them</t>
   </si>
   <si>
-    <t>How to choose a sleeping bag for your little one</t>
-  </si>
-  <si>
-    <t>Safely administering pain relief to your little one</t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -220,13 +196,16 @@
     <t>Why choose organic cotton for your baby?</t>
   </si>
   <si>
-    <t>How to choose a baby growsuit &amp; onesie?</t>
-  </si>
-  <si>
     <t>Small Rainbow Jumper</t>
   </si>
   <si>
     <t>CFrangipani Embroidered Dress</t>
+  </si>
+  <si>
+    <t>iti_7</t>
+  </si>
+  <si>
+    <t>iti_7@iti.com</t>
   </si>
 </sst>
 </file>
@@ -587,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC979B5-DE00-4264-9D5B-F48CC73FC465}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,15 +589,15 @@
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>3</v>
@@ -733,7 +712,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
@@ -761,7 +740,7 @@
     <row r="4" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
@@ -769,7 +748,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
@@ -778,7 +757,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -789,18 +768,18 @@
         <v>30215230</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -811,18 +790,18 @@
         <v>30215230</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
@@ -830,7 +809,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -857,7 +836,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
@@ -865,7 +844,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
@@ -873,23 +852,23 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -899,10 +878,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75306103-3AD1-4587-ACD9-B8DCD4545159}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,37 +891,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -966,18 +925,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -987,10 +946,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E552492-DBA6-4BB8-BC7E-197D254B633F}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,32 +959,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1054,19 +998,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1074,22 +1018,22 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C3" s="3"/>
       <c r="E3" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
@@ -1101,10 +1045,10 @@
         <v>5</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
@@ -1112,66 +1056,66 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
@@ -1185,10 +1129,10 @@
         <v>5</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
@@ -1196,16 +1140,16 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="40.5" x14ac:dyDescent="0.25">
@@ -1213,16 +1157,16 @@
         <v>4</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1234,7 +1178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C670E76-5AAF-41AD-B6C2-06048ED546A3}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1246,18 +1190,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>